<commit_message>
final consensus clustering definition.
</commit_message>
<xml_diff>
--- a/results/2016-12-02-annotation.xlsx
+++ b/results/2016-12-02-annotation.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
   <si>
     <t>sample_id</t>
   </si>
@@ -50,7 +50,7 @@
     <t>Pancreatic_Progenitor</t>
   </si>
   <si>
-    <t>Normal Stroma</t>
+    <t/>
   </si>
   <si>
     <t>PD2699_C4_1_YFP</t>
@@ -59,9 +59,6 @@
     <t>YFP</t>
   </si>
   <si>
-    <t>NA</t>
-  </si>
-  <si>
     <t>PD6422_C5_YFP</t>
   </si>
   <si>
@@ -78,9 +75,6 @@
   </si>
   <si>
     <t>PD6422_C5_BULK</t>
-  </si>
-  <si>
-    <t>Activated Stroma</t>
   </si>
   <si>
     <t>PD6499_C4_BULK</t>
@@ -604,15 +598,15 @@
         <v>11</v>
       </c>
       <c r="G3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
         <v>16</v>
-      </c>
-      <c r="B4" t="s">
-        <v>17</v>
       </c>
       <c r="C4" t="s">
         <v>14</v>
@@ -627,15 +621,15 @@
         <v>11</v>
       </c>
       <c r="G4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
         <v>18</v>
-      </c>
-      <c r="B5" t="s">
-        <v>19</v>
       </c>
       <c r="C5" t="s">
         <v>9</v>
@@ -655,10 +649,10 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C6" t="s">
         <v>14</v>
@@ -673,15 +667,15 @@
         <v>11</v>
       </c>
       <c r="G6" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C7" t="s">
         <v>9</v>
@@ -696,15 +690,15 @@
         <v>11</v>
       </c>
       <c r="G7" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C8" t="s">
         <v>9</v>
@@ -724,10 +718,10 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B9" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C9" t="s">
         <v>14</v>
@@ -742,15 +736,15 @@
         <v>11</v>
       </c>
       <c r="G9" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B10" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C10" t="s">
         <v>9</v>
@@ -770,10 +764,10 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B11" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C11" t="s">
         <v>14</v>
@@ -788,12 +782,12 @@
         <v>11</v>
       </c>
       <c r="G11" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B12" t="s">
         <v>8</v>
@@ -816,7 +810,7 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B13" t="s">
         <v>8</v>
@@ -834,15 +828,15 @@
         <v>11</v>
       </c>
       <c r="G13" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C14" t="s">
         <v>14</v>
@@ -857,15 +851,15 @@
         <v>11</v>
       </c>
       <c r="G14" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B15" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C15" t="s">
         <v>9</v>
@@ -880,15 +874,15 @@
         <v>11</v>
       </c>
       <c r="G15" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B16" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C16" t="s">
         <v>9</v>
@@ -908,10 +902,10 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B17" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C17" t="s">
         <v>14</v>
@@ -926,15 +920,15 @@
         <v>11</v>
       </c>
       <c r="G17" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B18" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C18" t="s">
         <v>14</v>
@@ -949,15 +943,15 @@
         <v>11</v>
       </c>
       <c r="G18" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B19" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C19" t="s">
         <v>9</v>
@@ -977,10 +971,10 @@
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B20" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C20" t="s">
         <v>9</v>
@@ -1000,10 +994,10 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B21" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C21" t="s">
         <v>14</v>
@@ -1018,15 +1012,15 @@
         <v>11</v>
       </c>
       <c r="G21" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B22" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C22" t="s">
         <v>14</v>
@@ -1041,15 +1035,15 @@
         <v>11</v>
       </c>
       <c r="G22" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B23" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C23" t="s">
         <v>14</v>
@@ -1064,15 +1058,15 @@
         <v>11</v>
       </c>
       <c r="G23" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B24" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C24" t="s">
         <v>9</v>
@@ -1084,18 +1078,18 @@
         <v>10</v>
       </c>
       <c r="F24" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G24" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B25" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C25" t="s">
         <v>14</v>
@@ -1110,15 +1104,15 @@
         <v>11</v>
       </c>
       <c r="G25" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B26" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C26" t="s">
         <v>14</v>
@@ -1133,15 +1127,15 @@
         <v>11</v>
       </c>
       <c r="G26" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B27" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C27" t="s">
         <v>9</v>
@@ -1161,10 +1155,10 @@
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B28" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C28" t="s">
         <v>14</v>
@@ -1179,15 +1173,15 @@
         <v>11</v>
       </c>
       <c r="G28" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B29" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C29" t="s">
         <v>14</v>
@@ -1202,15 +1196,15 @@
         <v>11</v>
       </c>
       <c r="G29" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B30" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C30" t="s">
         <v>14</v>
@@ -1225,15 +1219,15 @@
         <v>11</v>
       </c>
       <c r="G30" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B31" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C31" t="s">
         <v>9</v>
@@ -1253,10 +1247,10 @@
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B32" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C32" t="s">
         <v>14</v>
@@ -1271,15 +1265,15 @@
         <v>11</v>
       </c>
       <c r="G32" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B33" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C33" t="s">
         <v>9</v>
@@ -1291,18 +1285,18 @@
         <v>10</v>
       </c>
       <c r="F33" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G33" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B34" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C34" t="s">
         <v>9</v>
@@ -1322,10 +1316,10 @@
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B35" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C35" t="s">
         <v>9</v>
@@ -1345,10 +1339,10 @@
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B36" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C36" t="s">
         <v>14</v>
@@ -1363,15 +1357,15 @@
         <v>11</v>
       </c>
       <c r="G36" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B37" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C37" t="s">
         <v>9</v>

</xml_diff>